<commit_message>
feat: Change from multiple sheets to 1 sheet
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaflores/Code/Python/musicsorter/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67AB4F9-3C5C-5743-A015-5AF8FE6B858A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7967ACEF-450E-A64D-B930-2B5B54400671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="840" windowWidth="10940" windowHeight="18720" xr2:uid="{C39CD250-91A6-F147-AC42-3E99472E6AC6}"/>
+    <workbookView xWindow="15360" yWindow="580" windowWidth="22960" windowHeight="20940" xr2:uid="{C39CD250-91A6-F147-AC42-3E99472E6AC6}"/>
   </bookViews>
   <sheets>
     <sheet name="TECH HOUSE" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Date Added</t>
   </si>
@@ -122,24 +122,28 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=btPJPFnesV4</t>
+  </si>
+  <si>
+    <t>Playlist</t>
+  </si>
+  <si>
+    <t>TECH HOUSE</t>
+  </si>
+  <si>
+    <t>SUNSET HOUSE</t>
+  </si>
+  <si>
+    <t>BASS HOUSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,15 +183,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,7 +529,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,6 +538,7 @@
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -550,7 +554,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -562,8 +568,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -576,38 +585,101 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D4" s="5"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D5" s="5"/>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{6DF3C0B6-AC32-D145-96DA-AB33FA8485BB}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{71286DFC-8727-084A-A449-E9B147EC4D1A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{25C1F14D-C786-544A-8668-F95FA7F4EAD4}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{715DCD76-6761-2C41-A085-8525DC0F3EBD}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{A377C54B-306C-8144-8C15-710C5471EC1D}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{036B8B8B-98F2-1146-B7EA-3EFF0F806C27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -615,10 +687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079AC434-B1E5-6F4B-9BC9-9D6F5D80A9CB}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E3" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,9 +698,10 @@
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="35.1640625" customWidth="1"/>
     <col min="4" max="4" width="59.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,74 +714,45 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{25C1F14D-C786-544A-8668-F95FA7F4EAD4}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{715DCD76-6761-2C41-A085-8525DC0F3EBD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F2CB2C-6493-A643-9F4F-7D1DF9475270}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,9 +760,10 @@
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -731,82 +776,53 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{A377C54B-306C-8144-8C15-710C5471EC1D}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{036B8B8B-98F2-1146-B7EA-3EFF0F806C27}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>